<commit_message>
Update for end of August
</commit_message>
<xml_diff>
--- a/Thesis Cost Analysis.xlsx
+++ b/Thesis Cost Analysis.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="150" windowWidth="20115" windowHeight="7995"/>
+    <workbookView xWindow="240" yWindow="150" windowWidth="20115" windowHeight="7995" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -220,11 +220,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -567,7 +570,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:E30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+    <sheetView topLeftCell="A20" workbookViewId="0">
       <selection activeCell="A3" sqref="A3:E30"/>
     </sheetView>
   </sheetViews>
@@ -1065,12 +1068,66 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B2:B11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2" s="4"/>
+    </row>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B3" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B4" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B5" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B6" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B7" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B8" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B9" s="4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B10" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B11" s="4">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>